<commit_message>
TODO : read Statistical Region Merging, learns Sobel operation etc
added some documents
</commit_message>
<xml_diff>
--- a/mbak Raras/Port-Py/temp knowledge.xlsx
+++ b/mbak Raras/Port-Py/temp knowledge.xlsx
@@ -8,16 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Tugas Akhir\mbak Raras\Port-Py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14540C6C-D378-4E50-9554-834FA860E0E7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFD2BB2-FE72-4529-94AF-47F3A9905B34}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="4" r:id="rId1"/>
     <sheet name="SUM" sheetId="5" r:id="rId2"/>
+    <sheet name="Find" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Matlab</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3559,7 +3571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1BD7F89-8738-4A8B-8FB1-62F9821E088F}">
   <dimension ref="A1:DQ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CX1" workbookViewId="0">
+    <sheetView topLeftCell="CX1" workbookViewId="0">
       <selection activeCell="CX1" sqref="CX1"/>
     </sheetView>
   </sheetViews>
@@ -4807,4 +4819,1191 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C895271F-2A5A-47AA-86EF-D1D211F54E51}">
+  <dimension ref="A1:DM3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="DC1" workbookViewId="0">
+      <selection activeCell="DG3" sqref="DG3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:117" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>8</v>
+      </c>
+      <c r="I1">
+        <v>9</v>
+      </c>
+      <c r="J1">
+        <v>10</v>
+      </c>
+      <c r="K1">
+        <v>11</v>
+      </c>
+      <c r="L1">
+        <v>12</v>
+      </c>
+      <c r="M1">
+        <v>13</v>
+      </c>
+      <c r="N1">
+        <v>14</v>
+      </c>
+      <c r="O1">
+        <v>15</v>
+      </c>
+      <c r="P1">
+        <v>16</v>
+      </c>
+      <c r="Q1">
+        <v>17</v>
+      </c>
+      <c r="R1">
+        <v>18</v>
+      </c>
+      <c r="S1">
+        <v>19</v>
+      </c>
+      <c r="T1">
+        <v>20</v>
+      </c>
+      <c r="U1">
+        <v>21</v>
+      </c>
+      <c r="V1">
+        <v>22</v>
+      </c>
+      <c r="W1">
+        <v>23</v>
+      </c>
+      <c r="X1">
+        <v>24</v>
+      </c>
+      <c r="Y1">
+        <v>25</v>
+      </c>
+      <c r="Z1">
+        <v>26</v>
+      </c>
+      <c r="AA1">
+        <v>27</v>
+      </c>
+      <c r="AB1">
+        <v>28</v>
+      </c>
+      <c r="AC1">
+        <v>29</v>
+      </c>
+      <c r="AD1">
+        <v>30</v>
+      </c>
+      <c r="AE1">
+        <v>31</v>
+      </c>
+      <c r="AF1">
+        <v>32</v>
+      </c>
+      <c r="AG1">
+        <v>33</v>
+      </c>
+      <c r="AH1">
+        <v>34</v>
+      </c>
+      <c r="AI1">
+        <v>35</v>
+      </c>
+      <c r="AJ1">
+        <v>36</v>
+      </c>
+      <c r="AK1">
+        <v>37</v>
+      </c>
+      <c r="AL1">
+        <v>38</v>
+      </c>
+      <c r="AM1">
+        <v>39</v>
+      </c>
+      <c r="AN1">
+        <v>40</v>
+      </c>
+      <c r="AO1">
+        <v>41</v>
+      </c>
+      <c r="AP1">
+        <v>42</v>
+      </c>
+      <c r="AQ1">
+        <v>43</v>
+      </c>
+      <c r="AR1">
+        <v>44</v>
+      </c>
+      <c r="AS1">
+        <v>45</v>
+      </c>
+      <c r="AT1">
+        <v>46</v>
+      </c>
+      <c r="AU1">
+        <v>47</v>
+      </c>
+      <c r="AV1">
+        <v>48</v>
+      </c>
+      <c r="AW1">
+        <v>49</v>
+      </c>
+      <c r="AX1">
+        <v>50</v>
+      </c>
+      <c r="AY1">
+        <v>51</v>
+      </c>
+      <c r="AZ1">
+        <v>52</v>
+      </c>
+      <c r="BA1">
+        <v>53</v>
+      </c>
+      <c r="BB1">
+        <v>54</v>
+      </c>
+      <c r="BC1">
+        <v>55</v>
+      </c>
+      <c r="BD1">
+        <v>56</v>
+      </c>
+      <c r="BE1">
+        <v>57</v>
+      </c>
+      <c r="BF1">
+        <v>58</v>
+      </c>
+      <c r="BG1">
+        <v>59</v>
+      </c>
+      <c r="BH1">
+        <v>60</v>
+      </c>
+      <c r="BI1">
+        <v>61</v>
+      </c>
+      <c r="BJ1">
+        <v>62</v>
+      </c>
+      <c r="BK1">
+        <v>63</v>
+      </c>
+      <c r="BL1">
+        <v>64</v>
+      </c>
+      <c r="BM1">
+        <v>65</v>
+      </c>
+      <c r="BN1">
+        <v>66</v>
+      </c>
+      <c r="BO1">
+        <v>67</v>
+      </c>
+      <c r="BP1">
+        <v>68</v>
+      </c>
+      <c r="BQ1">
+        <v>69</v>
+      </c>
+      <c r="BR1">
+        <v>70</v>
+      </c>
+      <c r="BS1">
+        <v>71</v>
+      </c>
+      <c r="BT1">
+        <v>72</v>
+      </c>
+      <c r="BU1">
+        <v>73</v>
+      </c>
+      <c r="BV1">
+        <v>74</v>
+      </c>
+      <c r="BW1">
+        <v>75</v>
+      </c>
+      <c r="BX1">
+        <v>76</v>
+      </c>
+      <c r="BY1">
+        <v>77</v>
+      </c>
+      <c r="BZ1">
+        <v>78</v>
+      </c>
+      <c r="CA1">
+        <v>79</v>
+      </c>
+      <c r="CB1">
+        <v>80</v>
+      </c>
+      <c r="CC1">
+        <v>81</v>
+      </c>
+      <c r="CD1">
+        <v>82</v>
+      </c>
+      <c r="CE1">
+        <v>83</v>
+      </c>
+      <c r="CF1">
+        <v>84</v>
+      </c>
+      <c r="CG1">
+        <v>85</v>
+      </c>
+      <c r="CH1">
+        <v>86</v>
+      </c>
+      <c r="CI1">
+        <v>87</v>
+      </c>
+      <c r="CJ1">
+        <v>88</v>
+      </c>
+      <c r="CK1">
+        <v>89</v>
+      </c>
+      <c r="CL1">
+        <v>90</v>
+      </c>
+      <c r="CM1">
+        <v>91</v>
+      </c>
+      <c r="CN1">
+        <v>92</v>
+      </c>
+      <c r="CO1">
+        <v>93</v>
+      </c>
+      <c r="CP1">
+        <v>94</v>
+      </c>
+      <c r="CQ1">
+        <v>95</v>
+      </c>
+      <c r="CR1">
+        <v>96</v>
+      </c>
+      <c r="CS1">
+        <v>97</v>
+      </c>
+      <c r="CT1">
+        <v>98</v>
+      </c>
+      <c r="CU1">
+        <v>99</v>
+      </c>
+      <c r="CV1">
+        <v>100</v>
+      </c>
+      <c r="CW1">
+        <v>101</v>
+      </c>
+      <c r="CX1">
+        <v>102</v>
+      </c>
+      <c r="CY1">
+        <v>103</v>
+      </c>
+      <c r="CZ1">
+        <v>104</v>
+      </c>
+      <c r="DA1">
+        <v>105</v>
+      </c>
+      <c r="DB1">
+        <v>106</v>
+      </c>
+      <c r="DC1">
+        <v>107</v>
+      </c>
+      <c r="DD1">
+        <v>108</v>
+      </c>
+      <c r="DE1">
+        <v>109</v>
+      </c>
+      <c r="DF1">
+        <v>110</v>
+      </c>
+      <c r="DG1">
+        <v>111</v>
+      </c>
+      <c r="DH1">
+        <v>113</v>
+      </c>
+      <c r="DI1">
+        <v>114</v>
+      </c>
+      <c r="DJ1">
+        <v>115</v>
+      </c>
+      <c r="DK1">
+        <v>116</v>
+      </c>
+      <c r="DL1">
+        <v>117</v>
+      </c>
+      <c r="DM1">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:117" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
+      </c>
+      <c r="J2">
+        <v>9</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>11</v>
+      </c>
+      <c r="M2">
+        <v>12</v>
+      </c>
+      <c r="N2">
+        <v>13</v>
+      </c>
+      <c r="O2">
+        <v>14</v>
+      </c>
+      <c r="P2">
+        <v>15</v>
+      </c>
+      <c r="Q2">
+        <v>16</v>
+      </c>
+      <c r="R2">
+        <v>17</v>
+      </c>
+      <c r="S2">
+        <v>18</v>
+      </c>
+      <c r="T2">
+        <v>19</v>
+      </c>
+      <c r="U2">
+        <v>20</v>
+      </c>
+      <c r="V2">
+        <v>21</v>
+      </c>
+      <c r="W2">
+        <v>22</v>
+      </c>
+      <c r="X2">
+        <v>23</v>
+      </c>
+      <c r="Y2">
+        <v>24</v>
+      </c>
+      <c r="Z2">
+        <v>25</v>
+      </c>
+      <c r="AA2">
+        <v>26</v>
+      </c>
+      <c r="AB2">
+        <v>27</v>
+      </c>
+      <c r="AC2">
+        <v>28</v>
+      </c>
+      <c r="AD2">
+        <v>29</v>
+      </c>
+      <c r="AE2">
+        <v>30</v>
+      </c>
+      <c r="AF2">
+        <v>31</v>
+      </c>
+      <c r="AG2">
+        <v>32</v>
+      </c>
+      <c r="AH2">
+        <v>33</v>
+      </c>
+      <c r="AI2">
+        <v>34</v>
+      </c>
+      <c r="AJ2">
+        <v>35</v>
+      </c>
+      <c r="AK2">
+        <v>36</v>
+      </c>
+      <c r="AL2">
+        <v>37</v>
+      </c>
+      <c r="AM2">
+        <v>38</v>
+      </c>
+      <c r="AN2">
+        <v>39</v>
+      </c>
+      <c r="AO2">
+        <v>40</v>
+      </c>
+      <c r="AP2">
+        <v>41</v>
+      </c>
+      <c r="AQ2">
+        <v>42</v>
+      </c>
+      <c r="AR2">
+        <v>43</v>
+      </c>
+      <c r="AS2">
+        <v>44</v>
+      </c>
+      <c r="AT2">
+        <v>45</v>
+      </c>
+      <c r="AU2">
+        <v>46</v>
+      </c>
+      <c r="AV2">
+        <v>47</v>
+      </c>
+      <c r="AW2">
+        <v>48</v>
+      </c>
+      <c r="AX2">
+        <v>49</v>
+      </c>
+      <c r="AY2">
+        <v>50</v>
+      </c>
+      <c r="AZ2">
+        <v>51</v>
+      </c>
+      <c r="BA2">
+        <v>52</v>
+      </c>
+      <c r="BB2">
+        <v>53</v>
+      </c>
+      <c r="BC2">
+        <v>54</v>
+      </c>
+      <c r="BD2">
+        <v>55</v>
+      </c>
+      <c r="BE2">
+        <v>56</v>
+      </c>
+      <c r="BF2">
+        <v>57</v>
+      </c>
+      <c r="BG2">
+        <v>58</v>
+      </c>
+      <c r="BH2">
+        <v>59</v>
+      </c>
+      <c r="BI2">
+        <v>60</v>
+      </c>
+      <c r="BJ2">
+        <v>61</v>
+      </c>
+      <c r="BK2">
+        <v>62</v>
+      </c>
+      <c r="BL2">
+        <v>63</v>
+      </c>
+      <c r="BM2">
+        <v>64</v>
+      </c>
+      <c r="BN2">
+        <v>65</v>
+      </c>
+      <c r="BO2">
+        <v>66</v>
+      </c>
+      <c r="BP2">
+        <v>67</v>
+      </c>
+      <c r="BQ2">
+        <v>68</v>
+      </c>
+      <c r="BR2">
+        <v>69</v>
+      </c>
+      <c r="BS2">
+        <v>70</v>
+      </c>
+      <c r="BT2">
+        <v>71</v>
+      </c>
+      <c r="BU2">
+        <v>72</v>
+      </c>
+      <c r="BV2">
+        <v>73</v>
+      </c>
+      <c r="BW2">
+        <v>74</v>
+      </c>
+      <c r="BX2">
+        <v>75</v>
+      </c>
+      <c r="BY2">
+        <v>76</v>
+      </c>
+      <c r="BZ2">
+        <v>77</v>
+      </c>
+      <c r="CA2">
+        <v>78</v>
+      </c>
+      <c r="CB2">
+        <v>79</v>
+      </c>
+      <c r="CC2">
+        <v>80</v>
+      </c>
+      <c r="CD2">
+        <v>81</v>
+      </c>
+      <c r="CE2">
+        <v>82</v>
+      </c>
+      <c r="CF2">
+        <v>83</v>
+      </c>
+      <c r="CG2">
+        <v>84</v>
+      </c>
+      <c r="CH2">
+        <v>85</v>
+      </c>
+      <c r="CI2">
+        <v>86</v>
+      </c>
+      <c r="CJ2">
+        <v>87</v>
+      </c>
+      <c r="CK2">
+        <v>88</v>
+      </c>
+      <c r="CL2">
+        <v>89</v>
+      </c>
+      <c r="CM2">
+        <v>90</v>
+      </c>
+      <c r="CN2">
+        <v>91</v>
+      </c>
+      <c r="CO2">
+        <v>92</v>
+      </c>
+      <c r="CP2">
+        <v>93</v>
+      </c>
+      <c r="CQ2">
+        <v>94</v>
+      </c>
+      <c r="CR2">
+        <v>95</v>
+      </c>
+      <c r="CS2">
+        <v>96</v>
+      </c>
+      <c r="CT2">
+        <v>97</v>
+      </c>
+      <c r="CU2">
+        <v>98</v>
+      </c>
+      <c r="CV2">
+        <v>99</v>
+      </c>
+      <c r="CW2">
+        <v>100</v>
+      </c>
+      <c r="CX2">
+        <v>101</v>
+      </c>
+      <c r="CY2">
+        <v>102</v>
+      </c>
+      <c r="CZ2">
+        <v>103</v>
+      </c>
+      <c r="DA2">
+        <v>104</v>
+      </c>
+      <c r="DB2">
+        <v>105</v>
+      </c>
+      <c r="DC2">
+        <v>106</v>
+      </c>
+      <c r="DD2">
+        <v>107</v>
+      </c>
+      <c r="DE2">
+        <v>108</v>
+      </c>
+      <c r="DF2">
+        <v>109</v>
+      </c>
+      <c r="DG2">
+        <v>110</v>
+      </c>
+      <c r="DH2">
+        <v>112</v>
+      </c>
+      <c r="DI2">
+        <v>113</v>
+      </c>
+      <c r="DJ2">
+        <v>114</v>
+      </c>
+      <c r="DK2">
+        <v>115</v>
+      </c>
+      <c r="DL2">
+        <v>116</v>
+      </c>
+      <c r="DM2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:117" x14ac:dyDescent="0.3">
+      <c r="B3" t="str">
+        <f>IF((B1)=(B2+1), "BENER", "SALAH")</f>
+        <v>BENER</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:BN3" si="0">IF((C1)=(C2+1), "BENER", "SALAH")</f>
+        <v>BENER</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="N3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="P3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="Q3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="R3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="S3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="T3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="U3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="V3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="W3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="X3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="Y3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="Z3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AA3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AB3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AC3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AD3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AE3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AF3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AG3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AH3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AI3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AJ3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AK3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AL3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AM3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AN3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AO3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AP3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AQ3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AR3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AS3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AT3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AU3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AV3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AW3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AX3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AY3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="AZ3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="BA3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="BB3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="BC3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="BD3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="BE3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="BF3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="BG3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="BH3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="BI3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="BJ3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="BK3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="BL3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="BM3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="BN3" t="str">
+        <f t="shared" si="0"/>
+        <v>BENER</v>
+      </c>
+      <c r="BO3" t="str">
+        <f t="shared" ref="BO3:DM3" si="1">IF((BO1)=(BO2+1), "BENER", "SALAH")</f>
+        <v>BENER</v>
+      </c>
+      <c r="BP3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="BQ3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="BR3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="BS3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="BT3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="BU3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="BV3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="BW3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="BX3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="BY3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="BZ3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CA3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CB3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CC3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CD3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CE3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CF3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CG3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CH3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CI3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CJ3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CK3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CL3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CM3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CN3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CO3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CP3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CQ3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CR3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CS3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CT3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CU3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CV3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CW3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CX3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CY3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="CZ3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="DA3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="DB3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="DC3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="DD3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="DE3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="DF3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="DG3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="DH3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="DI3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="DJ3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="DK3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="DL3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+      <c r="DM3" t="str">
+        <f t="shared" si="1"/>
+        <v>BENER</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>